<commit_message>
mejoras en el mecanismo de registro de datos
</commit_message>
<xml_diff>
--- a/web/files/registro.xlsx
+++ b/web/files/registro.xlsx
@@ -575,7 +575,7 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
+      <selection pane="topLeft" activeCell="G22" activeCellId="0" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,7 +587,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="7.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.13"/>
@@ -1388,7 +1388,7 @@
       <c r="B45" s="11"/>
       <c r="C45" s="11"/>
       <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
+      <c r="E45" s="0"/>
       <c r="F45" s="12"/>
       <c r="G45" s="12"/>
       <c r="H45" s="12"/>
@@ -1487,7 +1487,7 @@
       <formula>ISBLANK(A13)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D6:L49">
+  <conditionalFormatting sqref="D6:L44 D46:L49 D45 F45:L45">
     <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
       <formula>-1</formula>
     </cfRule>
@@ -1499,7 +1499,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" error="Por favor.&#10;&#10;Recuerde que solo puede ingresar valores desde cero hasta #####" errorTitle="Error en el valor ingresado" operator="greaterThanOrEqual" prompt="Debe ingresar el total por dia para que la casilla se vuelva verde&#10;&#10;Cuando sea un dia sin abstecimiento por favor ingresar el valor de (-1)" promptTitle="Indicaciones generales" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D6:L49" type="whole">
+    <dataValidation allowBlank="true" error="Por favor.&#10;&#10;Recuerde que solo puede ingresar valores desde cero hasta #####" errorTitle="Error en el valor ingresado" operator="greaterThanOrEqual" prompt="Debe ingresar el total por dia para que la casilla se vuelva verde&#10;&#10;Cuando sea un dia sin abstecimiento por favor ingresar el valor de (-1)" promptTitle="Indicaciones generales" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D6:L44 D45 F45:L45 D46:L49" type="whole">
       <formula1>-1</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
prototipo final para archivo excel
</commit_message>
<xml_diff>
--- a/web/files/registro.xlsx
+++ b/web/files/registro.xlsx
@@ -49,16 +49,16 @@
     <t xml:space="preserve">Nombre</t>
   </si>
   <si>
+    <t xml:space="preserve">Lote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Existencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vencimiento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Consumo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Existencia</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lote</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vencimiento</t>
   </si>
   <si>
     <t xml:space="preserve">Cubiertos</t>
@@ -3524,8 +3524,8 @@
   </sheetPr>
   <dimension ref="A1:AI962"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="U15" activeCellId="0" sqref="U15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3533,9 +3533,9 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="12.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.42"/>
@@ -3547,7 +3547,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="20.56"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="18" min="17" style="2" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="true" outlineLevel="0" max="19" min="19" style="3" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="20" style="2" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="35" min="35" style="4" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="36" style="1" width="11.57"/>
@@ -3651,13 +3651,13 @@
         <v>15</v>
       </c>
       <c r="K5" s="16" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="L5" s="16" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="N5" s="16" t="s">
         <v>17</v>

</xml_diff>